<commit_message>
Supplementary Matherial and Manuscript update
Update of Supplementary Methods, Supplementary Tables, and Methods. Results for analysis of learning curves included.
</commit_message>
<xml_diff>
--- a/paper/supplementary tables.xlsx
+++ b/paper/supplementary tables.xlsx
@@ -8,17 +8,19 @@
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
-    <sheet name="Table S1" sheetId="2" r:id="rId2"/>
-    <sheet name="Table S2" sheetId="3" r:id="rId3"/>
-    <sheet name="Table S3" sheetId="4" r:id="rId4"/>
-    <sheet name="Table S4" sheetId="5" r:id="rId5"/>
-    <sheet name="Table S5" sheetId="6" r:id="rId6"/>
-    <sheet name="Table S6" sheetId="7" r:id="rId7"/>
-    <sheet name="Table S7" sheetId="8" r:id="rId8"/>
-    <sheet name="Table S8" sheetId="9" r:id="rId9"/>
-    <sheet name="Table S9" sheetId="10" r:id="rId10"/>
-    <sheet name="Table S10" sheetId="11" r:id="rId11"/>
-    <sheet name="Table S11" sheetId="12" r:id="rId12"/>
+    <sheet name="Supplementary Table S1" sheetId="2" r:id="rId2"/>
+    <sheet name="Supplementary Table S2" sheetId="3" r:id="rId3"/>
+    <sheet name="Supplementary Table S3" sheetId="4" r:id="rId4"/>
+    <sheet name="Supplementary Table S4" sheetId="5" r:id="rId5"/>
+    <sheet name="Supplementary Table S5" sheetId="6" r:id="rId6"/>
+    <sheet name="Supplementary Table S6" sheetId="7" r:id="rId7"/>
+    <sheet name="Supplementary Table S7" sheetId="8" r:id="rId8"/>
+    <sheet name="Supplementary Table S8" sheetId="9" r:id="rId9"/>
+    <sheet name="Supplementary Table S9" sheetId="10" r:id="rId10"/>
+    <sheet name="Supplementary Table S10" sheetId="11" r:id="rId11"/>
+    <sheet name="Supplementary Table S11" sheetId="12" r:id="rId12"/>
+    <sheet name="Supplementary Table S12" sheetId="13" r:id="rId13"/>
+    <sheet name="Supplementary Table S13" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -362,7 +364,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -383,7 +385,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Table S1</t>
+          <t>Supplementary Table S1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -395,7 +397,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Table S2</t>
+          <t>Supplementary Table S2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -407,7 +409,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Table S3</t>
+          <t>Supplementary Table S3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -419,7 +421,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Table S4</t>
+          <t>Supplementary Table S4</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -431,7 +433,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Table S5</t>
+          <t>Supplementary Table S5</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -443,19 +445,19 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Table S6</t>
+          <t>Supplementary Table S6</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Selection of machine learning algorithm parameters by cross-validation-mediated tuning.</t>
+          <t>Selection of machine learning algorithm hyper-parameters by cross-validation-mediated tuning.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Table S7</t>
+          <t>Supplementary Table S7</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -467,7 +469,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Table S8</t>
+          <t>Supplementary Table S8</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -479,34 +481,58 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Table S9</t>
+          <t>Supplementary Table S9</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Mean values of SHAP (Shapley additive explanations) variable importance statistic for the models of reduced diffusion capacity for CO and of diffusion capacity for CO &lt; 80% of reference. The table is available as a supplementary Excel file.</t>
+          <t>Mean values of SHAP (Shapley additive explanations) variable importance statistic for the models of reduced diffusion capacity for carbon monoxide and of diffusion capacity for carboon monoxide &lt; 80% of reference. The table is available as a supplementary Excel file.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Table S10</t>
+          <t>Supplementary Table S10</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Differences in chest computed tomography severity score (CTSS), and AI-determined lung opacity and high opacity in CovILD study participants with and without lung function testing (LFT) abnormalities. Numeric variariables are presented as medians with interquartile ranges (IQR) and ranges.</t>
+          <t>Correlations between chest computed tomography severity score, and AI-determined opacity and high opacity.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Table S11</t>
+          <t>Supplementary Table S11</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
+        <is>
+          <t>Differences in chest computed tomography severity score (CTSS), and AI-determined lung opacity and high opacity in CovILD study participants with and without ground glass opacities (GGO) and reticulation. Numeric variables are presented as medians with interquartile ranges (IQR) and ranges.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Supplementary Table S12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Differences in chest computed tomography severity score (CTSS), and AI-determined lung opacity and high opacity in CovILD study participants with and without lung function testing (LFT) abnormalities. Numeric variables are presented as medians with interquartile ranges (IQR) and ranges.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Supplementary Table S13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>Correlation of LFT variables with chest computed tomography severity score, and AI-determined opacity and high opacity.</t>
         </is>
@@ -1536,6 +1562,426 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Variable 1</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Variable 2</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Correlation coefficient</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Significance</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CTSS</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>opacity, AI</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>420</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ρ = 0.83 [0.77 - 0.88]</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CTSS</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>high opacity, AI</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>420</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ρ = 0.72 [0.65 - 0.79]</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>opacity, AI</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>high opacity, AI</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>420</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ρ = 0.86 [0.83 - 0.89]</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>CT abnormality</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Variable</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Abnormality absent</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Abnormality present</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Significance</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Effect size</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>GGO</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Observations, n</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>187</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>233</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>GGO</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CTSS, points</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0]
+range: 0 - 15
+complete: n = 187</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>7 [IQR: 3 - 12]
+range: 0 - 20
+complete: n = 233</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>r = 0.92</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>GGO</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>opacity, AI, % of lung</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0.01]
+range: 0 - 4.8
+complete: n = 187</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0.53 [IQR: 0.05 - 2.6]
+range: 0 - 37
+complete: n = 233</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>r = 0.75</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>GGO</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>high opacity, AI, % of lung</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0]
+range: 0 - 1
+complete: n = 187</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0.012 [IQR: 0 - 0.091]
+range: 0 - 3.1
+complete: n = 233</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>r = 0.55</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>reticulation</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Observations, n</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>213</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>207</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>reticulation</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CTSS, points</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0]
+range: 0 - 15
+complete: n = 213</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>7 [IQR: 3 - 13]
+range: 1 - 20
+complete: n = 207</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>r = 0.87</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>reticulation</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>opacity, AI, % of lung</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0.015]
+range: 0 - 18
+complete: n = 213</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0.59 [IQR: 0.08 - 3]
+range: 0 - 37
+complete: n = 207</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>r = 0.78</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>reticulation</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>high opacity, AI, % of lung</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0]
+range: 0 - 2.4
+complete: n = 213</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0.019 [IQR: 0 - 0.11]
+range: 0 - 3.1
+complete: n = 207</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>p &lt; 0.001</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>r = 0.61</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1969,7 +2415,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -6984,7 +7430,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>sigma = 0.01529346
+          <t>sigma = 0.0153
 C = 0.2</t>
         </is>
       </c>
@@ -7059,7 +7505,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>sigma = 0.01529346
+          <t>sigma = 0.0153
 C = 0.9</t>
         </is>
       </c>
@@ -7134,7 +7580,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>sigma = 0.01529346
+          <t>sigma = 0.0153
 C = 0.1</t>
         </is>
       </c>
@@ -7209,7 +7655,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>sigma = 0.01691549
+          <t>sigma = 0.0169
 C = 0.2</t>
         </is>
       </c>
@@ -7284,7 +7730,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>sigma = 0.01691549
+          <t>sigma = 0.0169
 C = 0.1</t>
         </is>
       </c>
@@ -7359,7 +7805,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>sigma = 0.01691549
+          <t>sigma = 0.0169
 C = 0.1</t>
         </is>
       </c>

</xml_diff>

<commit_message>
DLCO <80% predictions and DLCO values
Analysis of predictions of DLCO < 80% in observations with increasing DLCO values expressed as percentages of the patient's reference. Drop-out rates and frequency of LFT and CT abnormalities included in the manuscript text.
</commit_message>
<xml_diff>
--- a/paper/supplementary tables.xlsx
+++ b/paper/supplementary tables.xlsx
@@ -1611,7 +1611,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ρ = 0.83 [0.77 - 0.88]</t>
+          <t>ρ = 0.83 [0.78 - 0.88]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -2682,7 +2682,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2718,76 +2718,95 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2-month</t>
+          <t>all time points</t>
         </is>
       </c>
       <c r="B2">
-        <v>120</v>
+        <v>420</v>
       </c>
       <c r="C2">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="D2">
-        <v>71</v>
+        <v>234</v>
       </c>
       <c r="E2">
-        <v>22</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3-month</t>
+          <t>2-month</t>
         </is>
       </c>
       <c r="B3">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C3">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D3">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E3">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>6-month</t>
+          <t>3-month</t>
         </is>
       </c>
       <c r="B4">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D4">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E4">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2-month</t>
+          <t>6-month</t>
         </is>
       </c>
       <c r="B5">
+        <v>85</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>51</v>
+      </c>
+      <c r="E5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>12-month</t>
+        </is>
+      </c>
+      <c r="B6">
         <v>91</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>19</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>46</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>26</v>
       </c>
     </row>
@@ -4358,7 +4377,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4377,20 +4396,25 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>all time points</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>2-month follow-up</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>3-month follow-up</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>6-month follow-up</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>12-month follow-up</t>
         </is>
@@ -4409,23 +4433,29 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>62% (n = 259)
+complete: n = 420</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>71% (n = 85)
 complete: n = 120</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>57% (n = 71)
 complete: n = 124</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>64% (n = 54)
 complete: n = 85</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>54% (n = 49)
 complete: n = 91</t>
@@ -4445,23 +4475,29 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>55% (n = 233)
+complete: n = 420</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>69% (n = 83)
 complete: n = 120</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>53% (n = 66)
 complete: n = 124</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>52% (n = 44)
 complete: n = 85</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>44% (n = 40)
 complete: n = 91</t>
@@ -4481,23 +4517,29 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>49% (n = 207)
+complete: n = 420</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>51% (n = 61)
 complete: n = 120</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>48% (n = 60)
 complete: n = 124</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>55% (n = 47)
 complete: n = 85</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>43% (n = 39)
 complete: n = 91</t>
@@ -4517,23 +4559,29 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>5.5% (n = 23)
+complete: n = 420</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>11% (n = 13)
 complete: n = 120</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>6.5% (n = 8)
 complete: n = 124</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>1.2% (n = 1)
 complete: n = 85</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>1.1% (n = 1)
 complete: n = 91</t>
@@ -4553,23 +4601,29 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>8.1% (n = 34)
+complete: n = 420</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>10% (n = 12)
 complete: n = 120</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>5.6% (n = 7)
 complete: n = 124</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>8.2% (n = 7)
 complete: n = 85</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>8.8% (n = 8)
 complete: n = 91</t>
@@ -4588,27 +4642,34 @@
         </is>
       </c>
       <c r="C7" t="inlineStr">
+        <is>
+          <t>2 [IQR: 0 - 8]
+range: 0 - 20
+complete: n = 420</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>5 [IQR: 0 - 13]
 range: 0 - 20
 complete: n = 120</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>2 [IQR: 0 - 7.2]
 range: 0 - 18
 complete: n = 124</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>2 [IQR: 0 - 5]
 range: 0 - 15
 complete: n = 85</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>1 [IQR: 0 - 5]
 range: 0 - 15
@@ -4629,26 +4690,33 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>0.04 [IQR: 0 - 0.71]
+range: 0 - 37
+complete: n = 420</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>0.19 [IQR: 0 - 2.7]
 range: 0 - 37
 complete: n = 120</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>0.074 [IQR: 0 - 0.86]
 range: 0 - 22
 complete: n = 124</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>0.04 [IQR: 0 - 0.43]
 range: 0 - 12
 complete: n = 85</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 0.12]
 range: 0 - 6.2
@@ -4669,26 +4737,33 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>0 [IQR: 0 - 0.025]
+range: 0 - 3.1
+complete: n = 420</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>0.005 [IQR: 0 - 0.11]
 range: 0 - 3.1
 complete: n = 120</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>0.002 [IQR: 0 - 0.053]
 range: 0 - 2.4
 complete: n = 124</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 0.01]
 range: 0 - 0.46
 complete: n = 85</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 0.01]
 range: 0 - 0.11
@@ -4709,23 +4784,29 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>20% (n = 17)
+complete: n = 85</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>26% (n = 7)
 complete: n = 27</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>17% (n = 5)
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>30% (n = 3)
 complete: n = 10</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>11% (n = 2)
 complete: n = 19</t>
@@ -4745,23 +4826,29 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>14% (n = 12)
+complete: n = 85</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>22% (n = 6)
 complete: n = 27</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>14% (n = 4)
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>10% (n = 1)
 complete: n = 10</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>5.3% (n = 1)
 complete: n = 19</t>
@@ -4781,23 +4868,29 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>11% (n = 9)
+complete: n = 85</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>7.4% (n = 2)
 complete: n = 27</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>6.9% (n = 2)
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>30% (n = 3)
 complete: n = 10</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>11% (n = 2)
 complete: n = 19</t>
@@ -4817,23 +4910,29 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>2.4% (n = 2)
+complete: n = 85</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>3.7% (n = 1)
 complete: n = 27</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>3.4% (n = 1)
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>0% (n = 0)
 complete: n = 10</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>0% (n = 0)
 complete: n = 19</t>
@@ -4854,22 +4953,28 @@
       <c r="C14" t="inlineStr">
         <is>
           <t>0% (n = 0)
+complete: n = 85</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0% (n = 0)
 complete: n = 27</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>0% (n = 0)
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>0% (n = 0)
 complete: n = 10</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>0% (n = 0)
 complete: n = 19</t>
@@ -4888,27 +4993,34 @@
         </is>
       </c>
       <c r="C15" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0]
+range: 0 - 20
+complete: n = 85</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 1]
 range: 0 - 20
 complete: n = 27</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 0]
 range: 0 - 9
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 2.2]
 range: 0 - 5
 complete: n = 10</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 0]
 range: 0 - 3
@@ -4929,26 +5041,33 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>0 [IQR: 0 - 0.02]
+range: 0 - 14
+complete: n = 85</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>0 [IQR: 0 - 0.04]
 range: 0 - 14
 complete: n = 27</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 0.04]
 range: 0 - 1.2
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 0.025]
 range: 0 - 0.17
 complete: n = 10</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 0]
 range: 0 - 0.16
@@ -4969,26 +5088,33 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>0 [IQR: 0 - 0]
+range: 0 - 1.9
+complete: n = 85</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t>0 [IQR: 0 - 0.001]
 range: 0 - 1.9
 complete: n = 27</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 0]
 range: 0 - 0.12
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 0]
 range: 0 - 0.03
 complete: n = 10</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 0]
 range: 0 - 0.05
@@ -5009,23 +5135,29 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>65% (n = 151)
+complete: n = 234</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>80% (n = 57)
 complete: n = 71</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>61% (n = 40)
 complete: n = 66</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>57% (n = 29)
 complete: n = 51</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>54% (n = 25)
 complete: n = 46</t>
@@ -5045,23 +5177,29 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>59% (n = 137)
+complete: n = 234</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
           <t>79% (n = 56)
 complete: n = 71</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>56% (n = 37)
 complete: n = 66</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>49% (n = 25)
 complete: n = 51</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>41% (n = 19)
 complete: n = 46</t>
@@ -5081,23 +5219,29 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>50% (n = 117)
+complete: n = 234</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>55% (n = 39)
 complete: n = 71</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>52% (n = 34)
 complete: n = 66</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>47% (n = 24)
 complete: n = 51</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>43% (n = 20)
 complete: n = 46</t>
@@ -5117,23 +5261,29 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>5.6% (n = 13)
+complete: n = 234</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
           <t>9.9% (n = 7)
 complete: n = 71</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>9.1% (n = 6)
 complete: n = 66</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>0% (n = 0)
 complete: n = 51</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>0% (n = 0)
 complete: n = 46</t>
@@ -5153,23 +5303,29 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>6.4% (n = 15)
+complete: n = 234</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
           <t>7% (n = 5)
 complete: n = 71</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>7.6% (n = 5)
 complete: n = 66</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>5.9% (n = 3)
 complete: n = 51</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>4.3% (n = 2)
 complete: n = 46</t>
@@ -5188,27 +5344,34 @@
         </is>
       </c>
       <c r="C23" t="inlineStr">
+        <is>
+          <t>2 [IQR: 0 - 7]
+range: 0 - 20
+complete: n = 234</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
         <is>
           <t>6 [IQR: 1.5 - 12]
 range: 0 - 20
 complete: n = 71</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>2 [IQR: 0 - 5.8]
 range: 0 - 13
 complete: n = 66</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>1 [IQR: 0 - 4.5]
 range: 0 - 13
 complete: n = 51</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="G23" t="inlineStr">
         <is>
           <t>1 [IQR: 0 - 2.8]
 range: 0 - 13
@@ -5229,26 +5392,33 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t>0.04 [IQR: 0 - 0.53]
+range: 0 - 22
+complete: n = 234</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
           <t>0.21 [IQR: 0.0055 - 2]
 range: 0 - 22
 complete: n = 71</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>0.057 [IQR: 0 - 0.59]
 range: 0 - 11
 complete: n = 66</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>0.02 [IQR: 0 - 0.29]
 range: 0 - 12
 complete: n = 51</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 0.048]
 range: 0 - 2
@@ -5269,26 +5439,33 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t>0 [IQR: 0 - 0.014]
+range: 0 - 3.1
+complete: n = 234</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
           <t>0.005 [IQR: 0 - 0.053]
 range: 0 - 3.1
 complete: n = 71</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>5e-04 [IQR: 0 - 0.027]
 range: 0 - 2.4
 complete: n = 66</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 0]
 range: 0 - 0.46
 complete: n = 51</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="G25" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 0]
 range: 0 - 0.11
@@ -5309,23 +5486,29 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t>90% (n = 91)
+complete: n = 101</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
           <t>95% (n = 21)
 complete: n = 22</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>90% (n = 26)
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>92% (n = 22)
 complete: n = 24</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>85% (n = 22)
 complete: n = 26</t>
@@ -5345,23 +5528,29 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
+          <t>83% (n = 84)
+complete: n = 101</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
           <t>95% (n = 21)
 complete: n = 22</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>86% (n = 25)
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>75% (n = 18)
 complete: n = 24</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="G27" t="inlineStr">
         <is>
           <t>77% (n = 20)
 complete: n = 26</t>
@@ -5381,23 +5570,29 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
+          <t>80% (n = 81)
+complete: n = 101</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
           <t>91% (n = 20)
 complete: n = 22</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>83% (n = 24)
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>83% (n = 20)
 complete: n = 24</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="G28" t="inlineStr">
         <is>
           <t>65% (n = 17)
 complete: n = 26</t>
@@ -5417,23 +5612,29 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t>7.9% (n = 8)
+complete: n = 101</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
           <t>23% (n = 5)
 complete: n = 22</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>3.4% (n = 1)
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>4.2% (n = 1)
 complete: n = 24</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="G29" t="inlineStr">
         <is>
           <t>3.8% (n = 1)
 complete: n = 26</t>
@@ -5453,23 +5654,29 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t>19% (n = 19)
+complete: n = 101</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
           <t>32% (n = 7)
 complete: n = 22</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>6.9% (n = 2)
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>17% (n = 4)
 complete: n = 24</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="G30" t="inlineStr">
         <is>
           <t>23% (n = 6)
 complete: n = 26</t>
@@ -5488,27 +5695,34 @@
         </is>
       </c>
       <c r="C31" t="inlineStr">
+        <is>
+          <t>10 [IQR: 3 - 14]
+range: 0 - 20
+complete: n = 101</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
         <is>
           <t>14 [IQR: 10 - 15]
 range: 0 - 20
 complete: n = 22</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>10 [IQR: 5 - 15]
 range: 0 - 18
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="F31" t="inlineStr">
         <is>
           <t>6 [IQR: 2.8 - 10]
 range: 0 - 15
 complete: n = 24</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
+      <c r="G31" t="inlineStr">
         <is>
           <t>5 [IQR: 2 - 11]
 range: 0 - 15
@@ -5529,26 +5743,33 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
+          <t>0.68 [IQR: 0.054 - 3.7]
+range: 0 - 37
+complete: n = 101</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
           <t>5.8 [IQR: 0.34 - 9.3]
 range: 0 - 37
 complete: n = 22</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>1.9 [IQR: 0.39 - 6.8]
 range: 0 - 22
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>0.32 [IQR: 0.042 - 2]
 range: 0 - 6.7
 complete: n = 24</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="G32" t="inlineStr">
         <is>
           <t>0.28 [IQR: 0 - 0.67]
 range: 0 - 6.2
@@ -5569,26 +5790,33 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
+          <t>0.02 [IQR: 0 - 0.16]
+range: 0 - 2.1
+complete: n = 101</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
           <t>0.19 [IQR: 0.066 - 0.81]
 range: 0 - 2.1
 complete: n = 22</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>0.06 [IQR: 0.011 - 0.26]
 range: 0 - 1
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 0.02]
 range: 0 - 0.23
 complete: n = 24</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="G33" t="inlineStr">
         <is>
           <t>0.01 [IQR: 0 - 0.02]
 range: 0 - 0.11
@@ -5603,7 +5831,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5622,20 +5850,25 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>all time points</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>2-month follow-up</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>3-month follow-up</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>6-month follow-up</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>12-month follow-up</t>
         </is>
@@ -5653,27 +5886,34 @@
         </is>
       </c>
       <c r="C2" t="inlineStr">
+        <is>
+          <t>90 [IQR: 82 - 98]
+range: 46 - 130
+complete: n = 420</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>88 [IQR: 80 - 97]
 range: 46 - 130
 complete: n = 120</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>90 [IQR: 83 - 97]
 range: 54 - 120
 complete: n = 124</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>91 [IQR: 84 - 98]
 range: 50 - 120
 complete: n = 85</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>90 [IQR: 84 - 99]
 range: 55 - 120
@@ -5694,23 +5934,29 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>20% (n = 83)
+complete: n = 420</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>24% (n = 29)
 complete: n = 120</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>21% (n = 26)
 complete: n = 124</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>18% (n = 15)
 complete: n = 85</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>14% (n = 13)
 complete: n = 91</t>
@@ -5729,27 +5975,34 @@
         </is>
       </c>
       <c r="C4" t="inlineStr">
+        <is>
+          <t>93 [IQR: 83 - 100]
+range: 30 - 140
+complete: n = 420</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>92 [IQR: 82 - 100]
 range: 50 - 140
 complete: n = 120</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>92 [IQR: 82 - 100]
 range: 30 - 130
 complete: n = 124</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>94 [IQR: 84 - 100]
 range: 30 - 130
 complete: n = 85</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>95 [IQR: 84 - 110]
 range: 60 - 140
@@ -5770,23 +6023,29 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>18% (n = 77)
+complete: n = 420</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>20% (n = 24)
 complete: n = 120</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>21% (n = 26)
 complete: n = 124</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>15% (n = 13)
 complete: n = 85</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>15% (n = 14)
 complete: n = 91</t>
@@ -5805,27 +6064,34 @@
         </is>
       </c>
       <c r="C6" t="inlineStr">
+        <is>
+          <t>94 [IQR: 82 - 110]
+range: 31 - 140
+complete: n = 420</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>91 [IQR: 77 - 110]
 range: 44 - 140
 complete: n = 120</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>94 [IQR: 83 - 110]
 range: 31 - 140
 complete: n = 124</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>95 [IQR: 83 - 110]
 range: 32 - 140
 complete: n = 85</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>93 [IQR: 86 - 110]
 range: 48 - 130
@@ -5846,23 +6112,29 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>22% (n = 94)
+complete: n = 420</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>29% (n = 35)
 complete: n = 120</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>22% (n = 27)
 complete: n = 124</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>21% (n = 18)
 complete: n = 85</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>15% (n = 14)
 complete: n = 91</t>
@@ -5881,27 +6153,34 @@
         </is>
       </c>
       <c r="C8" t="inlineStr">
+        <is>
+          <t>94 [IQR: 86 - 100]
+range: 46 - 110
+complete: n = 85</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>95 [IQR: 87 - 100]
 range: 46 - 110
 complete: n = 27</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>94 [IQR: 87 - 100]
 range: 64 - 110
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>91 [IQR: 86 - 100]
 range: 64 - 110
 complete: n = 10</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>95 [IQR: 85 - 100]
 range: 72 - 110
@@ -5922,23 +6201,29 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>15% (n = 13)
+complete: n = 85</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>11% (n = 3)
 complete: n = 27</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>17% (n = 5)
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>10% (n = 1)
 complete: n = 10</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>21% (n = 4)
 complete: n = 19</t>
@@ -5957,27 +6242,34 @@
         </is>
       </c>
       <c r="C10" t="inlineStr">
+        <is>
+          <t>96 [IQR: 86 - 100]
+range: 50 - 120
+complete: n = 85</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>94 [IQR: 86 - 100]
 range: 50 - 110
 complete: n = 27</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>98 [IQR: 87 - 100]
 range: 65 - 120
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>95 [IQR: 85 - 100]
 range: 70 - 110
 complete: n = 10</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>96 [IQR: 88 - 100]
 range: 72 - 110
@@ -5998,23 +6290,29 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>13% (n = 11)
+complete: n = 85</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>11% (n = 3)
 complete: n = 27</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>14% (n = 4)
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>10% (n = 1)
 complete: n = 10</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>16% (n = 3)
 complete: n = 19</t>
@@ -6033,27 +6331,34 @@
         </is>
       </c>
       <c r="C12" t="inlineStr">
+        <is>
+          <t>100 [IQR: 92 - 110]
+range: 52 - 140
+complete: n = 85</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
         <is>
           <t>110 [IQR: 91 - 120]
 range: 52 - 140
 complete: n = 27</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>100 [IQR: 96 - 110]
 range: 69 - 130
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>99 [IQR: 89 - 110]
 range: 77 - 130
 complete: n = 10</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>98 [IQR: 92 - 110]
 range: 74 - 120
@@ -6074,23 +6379,29 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>12% (n = 10)
+complete: n = 85</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>15% (n = 4)
 complete: n = 27</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>10% (n = 3)
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>20% (n = 2)
 complete: n = 10</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>5.3% (n = 1)
 complete: n = 19</t>
@@ -6109,27 +6420,34 @@
         </is>
       </c>
       <c r="C14" t="inlineStr">
+        <is>
+          <t>90 [IQR: 82 - 98]
+range: 46 - 130
+complete: n = 234</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>87 [IQR: 80 - 96]
 range: 46 - 130
 complete: n = 71</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>90 [IQR: 84 - 98]
 range: 54 - 110
 complete: n = 66</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>96 [IQR: 84 - 99]
 range: 50 - 120
 complete: n = 51</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>91 [IQR: 85 - 99]
 range: 55 - 120
@@ -6150,23 +6468,29 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>18% (n = 41)
+complete: n = 234</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>24% (n = 17)
 complete: n = 71</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>17% (n = 11)
 complete: n = 66</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>16% (n = 8)
 complete: n = 51</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>11% (n = 5)
 complete: n = 46</t>
@@ -6185,27 +6509,34 @@
         </is>
       </c>
       <c r="C16" t="inlineStr">
+        <is>
+          <t>94 [IQR: 84 - 100]
+range: 30 - 140
+complete: n = 234</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
         <is>
           <t>92 [IQR: 83 - 100]
 range: 60 - 140
 complete: n = 71</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>92 [IQR: 85 - 100]
 range: 30 - 120
 complete: n = 66</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>97 [IQR: 85 - 110]
 range: 30 - 130
 complete: n = 51</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>95 [IQR: 87 - 110]
 range: 60 - 140
@@ -6226,23 +6557,29 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>15% (n = 36)
+complete: n = 234</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t>17% (n = 12)
 complete: n = 71</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>17% (n = 11)
 complete: n = 66</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>12% (n = 6)
 complete: n = 51</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>15% (n = 7)
 complete: n = 46</t>
@@ -6261,27 +6598,34 @@
         </is>
       </c>
       <c r="C18" t="inlineStr">
+        <is>
+          <t>96 [IQR: 84 - 110]
+range: 31 - 140
+complete: n = 234</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
         <is>
           <t>93 [IQR: 79 - 100]
 range: 52 - 120
 complete: n = 71</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>96 [IQR: 85 - 110]
 range: 31 - 140
 complete: n = 66</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>100 [IQR: 89 - 110]
 range: 32 - 140
 complete: n = 51</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>97 [IQR: 87 - 110]
 range: 54 - 130
@@ -6302,23 +6646,29 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>20% (n = 47)
+complete: n = 234</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
           <t>25% (n = 18)
 complete: n = 71</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>20% (n = 13)
 complete: n = 66</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>18% (n = 9)
 complete: n = 51</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>15% (n = 7)
 complete: n = 46</t>
@@ -6337,27 +6687,34 @@
         </is>
       </c>
       <c r="C20" t="inlineStr">
+        <is>
+          <t>86 [IQR: 77 - 93]
+range: 54 - 120
+complete: n = 101</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
         <is>
           <t>83 [IQR: 71 - 91]
 range: 58 - 110
 complete: n = 22</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>86 [IQR: 71 - 91]
 range: 54 - 120
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>87 [IQR: 80 - 91]
 range: 61 - 110
 complete: n = 24</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>86 [IQR: 83 - 93]
 range: 58 - 120
@@ -6378,23 +6735,29 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>29% (n = 29)
+complete: n = 101</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
           <t>41% (n = 9)
 complete: n = 22</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>34% (n = 10)
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>25% (n = 6)
 complete: n = 24</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>15% (n = 4)
 complete: n = 26</t>
@@ -6413,27 +6776,34 @@
         </is>
       </c>
       <c r="C22" t="inlineStr">
+        <is>
+          <t>88 [IQR: 79 - 98]
+range: 60 - 130
+complete: n = 101</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
         <is>
           <t>83 [IQR: 75 - 97]
 range: 62 - 120
 complete: n = 22</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>88 [IQR: 78 - 98]
 range: 60 - 130
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>88 [IQR: 83 - 95]
 range: 66 - 110
 complete: n = 24</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>94 [IQR: 83 - 99]
 range: 63 - 120
@@ -6454,23 +6824,29 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>30% (n = 30)
+complete: n = 101</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
           <t>41% (n = 9)
 complete: n = 22</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>38% (n = 11)
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>25% (n = 6)
 complete: n = 24</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="G23" t="inlineStr">
         <is>
           <t>15% (n = 4)
 complete: n = 26</t>
@@ -6489,27 +6865,34 @@
         </is>
       </c>
       <c r="C24" t="inlineStr">
+        <is>
+          <t>85 [IQR: 71 - 92]
+range: 44 - 130
+complete: n = 101</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
         <is>
           <t>76 [IQR: 58 - 87]
 range: 44 - 130
 complete: n = 22</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>84 [IQR: 72 - 90]
 range: 49 - 110
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>85 [IQR: 71 - 93]
 range: 50 - 110
 complete: n = 24</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>89 [IQR: 83 - 97]
 range: 48 - 120
@@ -6530,23 +6913,29 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t>37% (n = 37)
+complete: n = 101</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
           <t>59% (n = 13)
 complete: n = 22</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>38% (n = 11)
 complete: n = 29</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>29% (n = 7)
 complete: n = 24</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="G25" t="inlineStr">
         <is>
           <t>23% (n = 6)
 complete: n = 26</t>
@@ -6560,7 +6949,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6579,20 +6968,25 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>all time points</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>2-month follow-up</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>3-month follow-up</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>6-month follow-up</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>12-month follow-up</t>
         </is>
@@ -6613,704 +7007,826 @@
         <is>
           <t>0 [IQR: 0 - 1]
 range: 0 - 4
-complete: n = 120</t>
+complete: n = 420</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1]
+range: 0 - 4
+complete: n = 240</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 1]
 range: 0 - 3
-complete: n = 124</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+complete: n = 248</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1]
+range: 0 - 4
+complete: n = 170</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0]
+range: 0 - 4
+complete: n = 182</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CovILD cohort</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>dyspnea, mMRC &gt; 0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>33% (n = 139)
+complete: n = 420</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>45% (n = 108)
+complete: n = 240</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>34% (n = 84)
+complete: n = 248</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>27% (n = 46)
+complete: n = 170</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>22% (n = 40)
+complete: n = 182</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CovILD cohort</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>cough</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>16% (n = 68)
+complete: n = 420</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>18% (n = 44)
+complete: n = 240</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>17% (n = 42)
+complete: n = 248</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>13% (n = 22)
+complete: n = 170</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>15% (n = 28)
+complete: n = 182</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CovILD cohort</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>physical performance, ECOG, points</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1]
+range: 0 - 4
+complete: n = 420</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1 [IQR: 0 - 1]
+range: 0 - 4
+complete: n = 240</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0.5 [IQR: 0 - 1]
+range: 0 - 4
+complete: n = 248</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1]
+range: 0 - 1
+complete: n = 170</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1]
+range: 0 - 2
+complete: n = 182</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CovILD cohort</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>impaired physical performance, ECOG &gt; 0</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>44% (n = 185)
+complete: n = 420</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>53% (n = 128)
+complete: n = 240</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>50% (n = 124)
+complete: n = 248</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>33% (n = 56)
+complete: n = 170</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>34% (n = 62)
+complete: n = 182</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ambulatory</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>dyspnea rating, mMRC, points</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 1]
 range: 0 - 4
 complete: n = 85</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1.8]
+range: 0 - 4
+complete: n = 54</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1]
+range: 0 - 3
+complete: n = 58</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1]
+range: 0 - 1
+complete: n = 20</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0]
+range: 0 - 1
+complete: n = 38</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ambulatory</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>dyspnea, mMRC &gt; 0</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>36% (n = 31)
+complete: n = 85</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>44% (n = 24)
+complete: n = 54</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>38% (n = 22)
+complete: n = 58</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>40% (n = 8)
+complete: n = 20</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>21% (n = 8)
+complete: n = 38</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ambulatory</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>cough</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>22% (n = 19)
+complete: n = 85</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>22% (n = 12)
+complete: n = 54</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>24% (n = 14)
+complete: n = 58</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>20% (n = 4)
+complete: n = 20</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>21% (n = 8)
+complete: n = 38</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ambulatory</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>physical performance, ECOG, points</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1 [IQR: 0 - 1]
+range: 0 - 4
+complete: n = 85</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1 [IQR: 0 - 1]
+range: 0 - 2
+complete: n = 54</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1 [IQR: 0 - 1]
+range: 0 - 4
+complete: n = 58</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1]
+range: 0 - 1
+complete: n = 20</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1]
+range: 0 - 1
+complete: n = 38</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ambulatory</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>impaired physical performance, ECOG &gt; 0</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>52% (n = 44)
+complete: n = 85</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>59% (n = 32)
+complete: n = 54</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>59% (n = 34)
+complete: n = 58</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>40% (n = 8)
+complete: n = 20</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>37% (n = 14)
+complete: n = 38</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>moderate</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>dyspnea rating, mMRC, points</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1]
+range: 0 - 4
+complete: n = 234</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1]
+range: 0 - 4
+complete: n = 142</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1]
+range: 0 - 3
+complete: n = 132</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0.75]
+range: 0 - 3
+complete: n = 102</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 0]
 range: 0 - 4
-complete: n = 91</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>CovILD cohort</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
+complete: n = 92</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>moderate</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>dyspnea, mMRC &gt; 0</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>45% (n = 54)
-complete: n = 120</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>34% (n = 42)
-complete: n = 124</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>27% (n = 23)
-complete: n = 85</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>22% (n = 20)
-complete: n = 91</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>CovILD cohort</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>31% (n = 73)
+complete: n = 234</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>38% (n = 54)
+complete: n = 142</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>36% (n = 48)
+complete: n = 132</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>25% (n = 26)
+complete: n = 102</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>20% (n = 18)
+complete: n = 92</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>moderate</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>cough</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>18% (n = 22)
-complete: n = 120</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>17% (n = 21)
-complete: n = 124</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>13% (n = 11)
-complete: n = 85</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>15% (n = 35)
+complete: n = 234</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>17% (n = 24)
+complete: n = 142</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>15% (n = 20)
+complete: n = 132</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>12% (n = 12)
+complete: n = 102</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
         <is>
           <t>15% (n = 14)
-complete: n = 91</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>CovILD cohort</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
+complete: n = 92</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>moderate</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>physical performance, ECOG, points</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1]
+range: 0 - 3
+complete: n = 234</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1]
+range: 0 - 3
+complete: n = 142</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1]
+range: 0 - 1
+complete: n = 132</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0.75]
+range: 0 - 1
+complete: n = 102</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1]
+range: 0 - 1
+complete: n = 92</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>moderate</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>impaired physical performance, ECOG &gt; 0</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>36% (n = 84)
+complete: n = 234</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>44% (n = 62)
+complete: n = 142</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>41% (n = 54)
+complete: n = 132</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>25% (n = 26)
+complete: n = 102</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>28% (n = 26)
+complete: n = 92</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>severe</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>dyspnea rating, mMRC, points</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1]
+range: 0 - 4
+complete: n = 101</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
         <is>
           <t>1 [IQR: 0 - 1]
 range: 0 - 4
-complete: n = 120</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0.5 [IQR: 0 - 1]
+complete: n = 44</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0]
+range: 0 - 3
+complete: n = 58</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0.25]
 range: 0 - 4
-complete: n = 124</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
+complete: n = 48</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 1]
 range: 0 - 1
-complete: n = 85</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
+complete: n = 52</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>severe</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>dyspnea, mMRC &gt; 0</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>35% (n = 35)
+complete: n = 101</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>68% (n = 30)
+complete: n = 44</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>24% (n = 14)
+complete: n = 58</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>25% (n = 12)
+complete: n = 48</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>27% (n = 14)
+complete: n = 52</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>severe</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>cough</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>14% (n = 14)
+complete: n = 101</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>18% (n = 8)
+complete: n = 44</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>14% (n = 8)
+complete: n = 58</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>12% (n = 6)
+complete: n = 48</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>12% (n = 6)
+complete: n = 52</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>severe</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>physical performance, ECOG, points</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>1 [IQR: 0 - 1]
+range: 0 - 4
+complete: n = 101</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>1 [IQR: 1 - 1]
+range: 0 - 4
+complete: n = 44</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>1 [IQR: 0 - 1]
+range: 0 - 2
+complete: n = 58</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 1]
+range: 0 - 1
+complete: n = 48</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
         <is>
           <t>0 [IQR: 0 - 1]
 range: 0 - 2
-complete: n = 91</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>CovILD cohort</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>impaired physical performance, ECOG &gt; 0</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>53% (n = 64)
-complete: n = 120</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>50% (n = 62)
-complete: n = 124</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>33% (n = 28)
-complete: n = 85</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>34% (n = 31)
-complete: n = 91</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>ambulatory</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>dyspnea rating, mMRC, points</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>0 [IQR: 0 - 1.5]
-range: 0 - 4
-complete: n = 27</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>0 [IQR: 0 - 1]
-range: 0 - 3
-complete: n = 29</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0 [IQR: 0 - 1]
-range: 0 - 1
-complete: n = 10</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>0 [IQR: 0 - 0]
-range: 0 - 1
-complete: n = 19</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>ambulatory</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>dyspnea, mMRC &gt; 0</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>44% (n = 12)
-complete: n = 27</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>38% (n = 11)
-complete: n = 29</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>40% (n = 4)
-complete: n = 10</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>21% (n = 4)
-complete: n = 19</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>ambulatory</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>cough</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>22% (n = 6)
-complete: n = 27</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>24% (n = 7)
-complete: n = 29</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>20% (n = 2)
-complete: n = 10</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>21% (n = 4)
-complete: n = 19</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>ambulatory</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>physical performance, ECOG, points</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1 [IQR: 0 - 1]
-range: 0 - 2
-complete: n = 27</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>1 [IQR: 0 - 1]
-range: 0 - 4
-complete: n = 29</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>0 [IQR: 0 - 1]
-range: 0 - 1
-complete: n = 10</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>0 [IQR: 0 - 1]
-range: 0 - 1
-complete: n = 19</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>ambulatory</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>impaired physical performance, ECOG &gt; 0</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>59% (n = 16)
-complete: n = 27</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>59% (n = 17)
-complete: n = 29</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>40% (n = 4)
-complete: n = 10</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>37% (n = 7)
-complete: n = 19</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>moderate</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>dyspnea rating, mMRC, points</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>0 [IQR: 0 - 1]
-range: 0 - 4
-complete: n = 71</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>0 [IQR: 0 - 1]
-range: 0 - 3
-complete: n = 66</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>0 [IQR: 0 - 0.5]
-range: 0 - 3
-complete: n = 51</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>0 [IQR: 0 - 0]
-range: 0 - 4
-complete: n = 46</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>moderate</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>dyspnea, mMRC &gt; 0</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>38% (n = 27)
-complete: n = 71</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>36% (n = 24)
-complete: n = 66</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>25% (n = 13)
-complete: n = 51</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>20% (n = 9)
-complete: n = 46</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>moderate</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>cough</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>17% (n = 12)
-complete: n = 71</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>15% (n = 10)
-complete: n = 66</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>12% (n = 6)
-complete: n = 51</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>15% (n = 7)
-complete: n = 46</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>moderate</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>physical performance, ECOG, points</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>0 [IQR: 0 - 1]
-range: 0 - 3
-complete: n = 71</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>0 [IQR: 0 - 1]
-range: 0 - 1
-complete: n = 66</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>0 [IQR: 0 - 0.5]
-range: 0 - 1
-complete: n = 51</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>0 [IQR: 0 - 1]
-range: 0 - 1
-complete: n = 46</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>moderate</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>impaired physical performance, ECOG &gt; 0</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>44% (n = 31)
-complete: n = 71</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>41% (n = 27)
-complete: n = 66</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>25% (n = 13)
-complete: n = 51</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>28% (n = 13)
-complete: n = 46</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>severe</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>dyspnea rating, mMRC, points</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>1 [IQR: 0 - 1]
-range: 0 - 4
-complete: n = 22</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>0 [IQR: 0 - 0]
-range: 0 - 3
-complete: n = 29</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>0 [IQR: 0 - 0.25]
-range: 0 - 4
-complete: n = 24</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>0 [IQR: 0 - 0.75]
-range: 0 - 1
-complete: n = 26</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>severe</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>dyspnea, mMRC &gt; 0</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>68% (n = 15)
-complete: n = 22</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>24% (n = 7)
-complete: n = 29</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>25% (n = 6)
-complete: n = 24</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>27% (n = 7)
-complete: n = 26</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>severe</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>cough</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>18% (n = 4)
-complete: n = 22</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>14% (n = 4)
-complete: n = 29</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>12% (n = 3)
-complete: n = 24</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>12% (n = 3)
-complete: n = 26</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>severe</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>physical performance, ECOG, points</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>1 [IQR: 1 - 1]
-range: 0 - 4
-complete: n = 22</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>1 [IQR: 0 - 1]
-range: 0 - 2
-complete: n = 29</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>0 [IQR: 0 - 1]
-range: 0 - 1
-complete: n = 24</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>0 [IQR: 0 - 1]
-range: 0 - 2
-complete: n = 26</t>
+complete: n = 52</t>
         </is>
       </c>
     </row>
@@ -7327,26 +7843,32 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>77% (n = 17)
-complete: n = 22</t>
+          <t>56% (n = 57)
+complete: n = 101</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>62% (n = 18)
-complete: n = 29</t>
+          <t>77% (n = 34)
+complete: n = 44</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>46% (n = 11)
-complete: n = 24</t>
+          <t>62% (n = 36)
+complete: n = 58</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>42% (n = 11)
-complete: n = 26</t>
+          <t>46% (n = 22)
+complete: n = 48</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>42% (n = 22)
+complete: n = 52</t>
         </is>
       </c>
     </row>

</xml_diff>